<commit_message>
Atualização de scripts e planilha.
</commit_message>
<xml_diff>
--- a/scripts.xlsx
+++ b/scripts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos\Downloads\GPA\ebitacoatiara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GPA2025\ebitacoatiara\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C211171-6187-4164-9986-D57ED8B00307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C599E50-F4AF-451C-8266-4A22D8C0D1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F2648B7-5F5B-42DB-AD00-937C0D6B140B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NOME DO ARQUIVO</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>OBSERVAÇÕES</t>
+  </si>
+  <si>
+    <t>script000.py</t>
+  </si>
+  <si>
+    <t>Arquivo contendo funções gerais úteis nos demais scripts</t>
+  </si>
+  <si>
+    <t>script001.py</t>
+  </si>
+  <si>
+    <t>Carrega os dados de Itacoatiara e salva esses dados em arquivos separados</t>
   </si>
 </sst>
 </file>
@@ -98,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -394,13 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AB5883-CE8B-4BC7-95E9-D4403D0BF2CF}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -411,6 +428,22 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>